<commit_message>
changes in ms report 09/07/25
</commit_message>
<xml_diff>
--- a/public/data/Accrual vs. Actual Variance Report.xlsx
+++ b/public/data/Accrual vs. Actual Variance Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Karthik\Files\Proposals\Fresenius\Report Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New Task\MS_Report\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072C72A6-2C27-4D6D-B16E-03C8F2A302A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1434B070-79E1-4286-A4D7-7D2BA974C934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{4F2F02AC-2824-49F7-8931-77FA8E4E985F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4F2F02AC-2824-49F7-8931-77FA8E4E985F}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Design" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
-  <si>
-    <t>Accrual vs. Actual Variance Report</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Variance $</t>
   </si>
@@ -50,9 +47,6 @@
     <t>Aminomix 1 Novum</t>
   </si>
   <si>
-    <t>Run by: Admin</t>
-  </si>
-  <si>
     <t>Page 1 of 1</t>
   </si>
   <si>
@@ -117,15 +111,6 @@
   </si>
   <si>
     <t>Aminomix Rebate 2025</t>
-  </si>
-  <si>
-    <t>Program</t>
-  </si>
-  <si>
-    <t>Period</t>
-  </si>
-  <si>
-    <t>Q12025</t>
   </si>
 </sst>
 </file>
@@ -135,20 +120,13 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -200,19 +178,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="6" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -221,13 +192,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -243,70 +216,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>759254</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Fresenius Kabi">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E41C322-BA2E-4067-B88D-61E06F9155A1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect t="32911" b="31646"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="679450" y="0"/>
-          <a:ext cx="689404" cy="184150"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -626,178 +535,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8BB165-B51C-4A30-A6BF-DFB0F1C31B6F}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.90625" customWidth="1"/>
-    <col min="4" max="4" width="18.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" customWidth="1"/>
-    <col min="7" max="7" width="19.08984375" customWidth="1"/>
-    <col min="8" max="8" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2" t="s">
+      <c r="N1" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="8">
+        <v>45658</v>
+      </c>
+      <c r="H2" s="8">
+        <v>45747</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1">
+        <v>287230</v>
+      </c>
+      <c r="L2" s="1">
+        <v>263418</v>
+      </c>
+      <c r="M2" s="9">
+        <f>K2-L2</f>
+        <v>23812</v>
+      </c>
+      <c r="N2" s="10">
+        <f>(M2/L2)*100</f>
+        <v>9.0396252344183008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="11">
-        <v>45658</v>
-      </c>
-      <c r="I9" s="11">
-        <v>45747</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="1">
-        <v>287230</v>
-      </c>
-      <c r="M9" s="1">
-        <v>263418</v>
-      </c>
-      <c r="N9" s="12">
-        <f>L9-M9</f>
-        <v>23812</v>
-      </c>
-      <c r="O9" s="13">
-        <f>(N9/M9)*100</f>
-        <v>9.0396252344183008</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
+    <row r="9" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="C11:G11"/>
+  <mergeCells count="1">
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>